<commit_message>
SA extra explanations, excell
</commit_message>
<xml_diff>
--- a/Sensitivity Analysis/Sensitivity Analysis.xlsx
+++ b/Sensitivity Analysis/Sensitivity Analysis.xlsx
@@ -5,30 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inosoft_04\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarzaminDigital\Desktop\PAPER\MATLAB\Sensitivity Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7634B727-585D-41D4-80BB-033AB330B7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575747CB-6B1E-4DB1-809B-960BA57D2371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{20D8FD35-607E-478C-A7D4-3B7328D000D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{20D8FD35-607E-478C-A7D4-3B7328D000D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Machine" sheetId="1" r:id="rId1"/>
     <sheet name="Jobs" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -80,13 +72,32 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -103,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,11 +122,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -123,9 +153,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3996,7 +4058,7 @@
   <dimension ref="A1:Z73"/>
   <sheetViews>
     <sheetView topLeftCell="L4" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4014,23 +4076,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -4252,23 +4314,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -4762,23 +4824,23 @@
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
       <c r="Q28" s="1">
         <v>6</v>
       </c>
@@ -6109,7 +6171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B710F4EF-F548-4993-AD33-7EBEF4E379ED}">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
@@ -6121,23 +6183,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -6573,23 +6635,23 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
       <c r="Q14" s="1">
         <v>42</v>
       </c>
@@ -7220,23 +7282,23 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -8146,4 +8208,604 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C8CAFA-AC4C-47BF-B788-C4EF00656907}">
+  <dimension ref="I10:Y27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="10" spans="9:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I11" s="4">
+        <v>31.17</v>
+      </c>
+      <c r="J11" s="4">
+        <v>117.33</v>
+      </c>
+      <c r="K11" s="4">
+        <v>71.33</v>
+      </c>
+      <c r="T11" s="5">
+        <v>26.08</v>
+      </c>
+      <c r="U11" s="5">
+        <v>97.08</v>
+      </c>
+      <c r="V11" s="5">
+        <v>75.67</v>
+      </c>
+    </row>
+    <row r="12" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I12" s="6">
+        <v>26.08</v>
+      </c>
+      <c r="J12" s="6">
+        <v>97.08</v>
+      </c>
+      <c r="K12" s="6">
+        <v>75.67</v>
+      </c>
+      <c r="L12" s="7">
+        <f>-(I11-I12)/I11</f>
+        <v>-0.16329804299005465</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" ref="M12:N24" si="0">-(J11-J12)/J11</f>
+        <v>-0.17259013040143187</v>
+      </c>
+      <c r="N12" s="7">
+        <f t="shared" si="0"/>
+        <v>6.0843964671246371E-2</v>
+      </c>
+      <c r="T12" s="8">
+        <v>28.58</v>
+      </c>
+      <c r="U12" s="8">
+        <v>120.83</v>
+      </c>
+      <c r="V12" s="8">
+        <v>85.67</v>
+      </c>
+      <c r="W12" s="7">
+        <f>-(T12-T11)/T11</f>
+        <v>-9.5858895705521474E-2</v>
+      </c>
+      <c r="X12" s="7">
+        <f t="shared" ref="X12:Y24" si="1">-(U12-U11)/U11</f>
+        <v>-0.2446435929130614</v>
+      </c>
+      <c r="Y12" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.13215276860050218</v>
+      </c>
+    </row>
+    <row r="13" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I13" s="6">
+        <v>13.06</v>
+      </c>
+      <c r="J13" s="6">
+        <v>54.44</v>
+      </c>
+      <c r="K13" s="6">
+        <v>79.5</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" ref="L13:L24" si="2">-(I12-I13)/I12</f>
+        <v>-0.49923312883435578</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.43922538112896581</v>
+      </c>
+      <c r="N13" s="7">
+        <f t="shared" si="0"/>
+        <v>5.0614510373992311E-2</v>
+      </c>
+      <c r="T13" s="8">
+        <v>31.08</v>
+      </c>
+      <c r="U13" s="8">
+        <v>150</v>
+      </c>
+      <c r="V13" s="8">
+        <v>95.67</v>
+      </c>
+      <c r="W13" s="7">
+        <f t="shared" ref="W13:W24" si="3">-(T13-T12)/T12</f>
+        <v>-8.7473757872638211E-2</v>
+      </c>
+      <c r="X13" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.24141355623603411</v>
+      </c>
+      <c r="Y13" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.1167269756040621</v>
+      </c>
+    </row>
+    <row r="14" spans="9:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="9">
+        <v>13.17</v>
+      </c>
+      <c r="J14" s="9">
+        <v>53.6</v>
+      </c>
+      <c r="K14" s="9">
+        <v>79.64</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="2"/>
+        <v>8.4226646248085311E-3</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.5429831006612717E-2</v>
+      </c>
+      <c r="N14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.7610062893081832E-3</v>
+      </c>
+      <c r="T14" s="10">
+        <v>28.97</v>
+      </c>
+      <c r="U14" s="10">
+        <v>154.63</v>
+      </c>
+      <c r="V14" s="10">
+        <v>108.53</v>
+      </c>
+      <c r="W14" s="7">
+        <f t="shared" si="3"/>
+        <v>6.7889317889317874E-2</v>
+      </c>
+      <c r="X14" s="7">
+        <f t="shared" si="1"/>
+        <v>-3.0866666666666636E-2</v>
+      </c>
+      <c r="Y14" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.13442040347026235</v>
+      </c>
+    </row>
+    <row r="15" spans="9:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12">
+        <f>SUM(L12:L14)/3</f>
+        <v>-0.21803616906653397</v>
+      </c>
+      <c r="M15" s="12">
+        <f t="shared" ref="M15:N15" si="4">SUM(M12:M14)/3</f>
+        <v>-0.20908178084567017</v>
+      </c>
+      <c r="N15" s="12">
+        <f t="shared" si="4"/>
+        <v>3.773982711151562E-2</v>
+      </c>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="12">
+        <f>SUM(W12:W14)/3</f>
+        <v>-3.8481111896280611E-2</v>
+      </c>
+      <c r="X15" s="12">
+        <f t="shared" ref="X15:Y15" si="5">SUM(X12:X14)/3</f>
+        <v>-0.17230793860525404</v>
+      </c>
+      <c r="Y15" s="12">
+        <f t="shared" si="5"/>
+        <v>-0.12776671589160887</v>
+      </c>
+    </row>
+    <row r="16" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I16" s="6">
+        <v>20.67</v>
+      </c>
+      <c r="J16" s="6">
+        <v>152</v>
+      </c>
+      <c r="K16" s="6">
+        <v>154.78</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="T16" s="6">
+        <v>16.53</v>
+      </c>
+      <c r="U16" s="6">
+        <v>118.86</v>
+      </c>
+      <c r="V16" s="6">
+        <v>150.66999999999999</v>
+      </c>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+    </row>
+    <row r="17" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I17" s="6">
+        <v>16.53</v>
+      </c>
+      <c r="J17" s="6">
+        <v>118.86</v>
+      </c>
+      <c r="K17" s="6">
+        <v>150.66999999999999</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.20029027576197389</v>
+      </c>
+      <c r="M17" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.21802631578947368</v>
+      </c>
+      <c r="N17" s="7">
+        <f t="shared" si="0"/>
+        <v>-2.6553818322780809E-2</v>
+      </c>
+      <c r="T17" s="6">
+        <v>17.11</v>
+      </c>
+      <c r="U17" s="6">
+        <v>128.79</v>
+      </c>
+      <c r="V17" s="6">
+        <v>157.47</v>
+      </c>
+      <c r="W17" s="7">
+        <f t="shared" si="3"/>
+        <v>-3.5087719298245508E-2</v>
+      </c>
+      <c r="X17" s="7">
+        <f t="shared" si="1"/>
+        <v>-8.3543664815749555E-2</v>
+      </c>
+      <c r="Y17" s="7">
+        <f t="shared" si="1"/>
+        <v>-4.5131744872901121E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I18" s="6">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="J18" s="6">
+        <v>122.19</v>
+      </c>
+      <c r="K18" s="6">
+        <v>148.75</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="2"/>
+        <v>3.2062915910465672E-2</v>
+      </c>
+      <c r="M18" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8016153457849555E-2</v>
+      </c>
+      <c r="N18" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.2743080905289625E-2</v>
+      </c>
+      <c r="T18" s="6">
+        <v>18.77</v>
+      </c>
+      <c r="U18" s="6">
+        <v>154.33000000000001</v>
+      </c>
+      <c r="V18" s="6">
+        <v>156.19999999999999</v>
+      </c>
+      <c r="W18" s="7">
+        <f t="shared" si="3"/>
+        <v>-9.7019286966686158E-2</v>
+      </c>
+      <c r="X18" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.19830732199704962</v>
+      </c>
+      <c r="Y18" s="7">
+        <f t="shared" si="1"/>
+        <v>8.0650282593510529E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="9:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="9">
+        <v>15.67</v>
+      </c>
+      <c r="J19" s="9">
+        <v>115.7</v>
+      </c>
+      <c r="K19" s="9">
+        <v>152.72999999999999</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="2"/>
+        <v>-8.1477139507620103E-2</v>
+      </c>
+      <c r="M19" s="7">
+        <f t="shared" si="0"/>
+        <v>-5.3114002782551725E-2</v>
+      </c>
+      <c r="N19" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6756302521008333E-2</v>
+      </c>
+      <c r="T19" s="9">
+        <v>18.72</v>
+      </c>
+      <c r="U19" s="9">
+        <v>155.88</v>
+      </c>
+      <c r="V19" s="9">
+        <v>167.98</v>
+      </c>
+      <c r="W19" s="7">
+        <f t="shared" si="3"/>
+        <v>2.6638252530634368E-3</v>
+      </c>
+      <c r="X19" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.0043413464653553E-2</v>
+      </c>
+      <c r="Y19" s="7">
+        <f t="shared" si="1"/>
+        <v>-7.5416133162612045E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="9:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12">
+        <f>SUM(L17:L19)/3</f>
+        <v>-8.3234833119709431E-2</v>
+      </c>
+      <c r="M20" s="12">
+        <f t="shared" ref="M20:N20" si="6">SUM(M17:M19)/3</f>
+        <v>-8.1041388371391951E-2</v>
+      </c>
+      <c r="N20" s="12">
+        <f t="shared" si="6"/>
+        <v>-4.1801989023540339E-3</v>
+      </c>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="12">
+        <f>SUM(W17:W19)/3</f>
+        <v>-4.3147727003956075E-2</v>
+      </c>
+      <c r="X20" s="12">
+        <f t="shared" ref="X20:Y20" si="7">SUM(X17:X19)/3</f>
+        <v>-9.7298133425817571E-2</v>
+      </c>
+      <c r="Y20" s="12">
+        <f t="shared" si="7"/>
+        <v>-3.7494283258720708E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I21" s="6">
+        <v>42.65</v>
+      </c>
+      <c r="J21" s="6">
+        <v>667.43</v>
+      </c>
+      <c r="K21" s="6">
+        <v>372.14</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="T21" s="6">
+        <v>36.33</v>
+      </c>
+      <c r="U21" s="6">
+        <v>550.16</v>
+      </c>
+      <c r="V21" s="6">
+        <v>400.43</v>
+      </c>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+    </row>
+    <row r="22" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I22" s="6">
+        <v>36.33</v>
+      </c>
+      <c r="J22" s="6">
+        <v>550.16</v>
+      </c>
+      <c r="K22" s="6">
+        <v>400.43</v>
+      </c>
+      <c r="L22" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.1481828839390387</v>
+      </c>
+      <c r="M22" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.17570381912709945</v>
+      </c>
+      <c r="N22" s="7">
+        <f t="shared" si="0"/>
+        <v>7.6019777503090288E-2</v>
+      </c>
+      <c r="T22" s="6">
+        <v>38.4</v>
+      </c>
+      <c r="U22" s="6">
+        <v>613.33000000000004</v>
+      </c>
+      <c r="V22" s="6">
+        <v>411.68</v>
+      </c>
+      <c r="W22" s="7">
+        <f t="shared" si="3"/>
+        <v>-5.6977704376548317E-2</v>
+      </c>
+      <c r="X22" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.11482114294023571</v>
+      </c>
+      <c r="Y22" s="7">
+        <f t="shared" si="1"/>
+        <v>-2.8094798092051045E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="I23" s="6">
+        <v>31.89</v>
+      </c>
+      <c r="J23" s="6">
+        <v>534.96</v>
+      </c>
+      <c r="K23" s="6">
+        <v>395.36</v>
+      </c>
+      <c r="L23" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.12221304706853835</v>
+      </c>
+      <c r="M23" s="7">
+        <f t="shared" si="0"/>
+        <v>-2.7628326305074766E-2</v>
+      </c>
+      <c r="N23" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.2661389006817654E-2</v>
+      </c>
+      <c r="T23" s="6">
+        <v>39.159999999999997</v>
+      </c>
+      <c r="U23" s="6">
+        <v>632.36</v>
+      </c>
+      <c r="V23" s="6">
+        <v>416.87</v>
+      </c>
+      <c r="W23" s="7">
+        <f t="shared" si="3"/>
+        <v>-1.9791666666666617E-2</v>
+      </c>
+      <c r="X23" s="7">
+        <f t="shared" si="1"/>
+        <v>-3.1027342539905061E-2</v>
+      </c>
+      <c r="Y23" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.2606879129420904E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="9:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="9">
+        <v>27.31</v>
+      </c>
+      <c r="J24" s="9">
+        <v>481.13</v>
+      </c>
+      <c r="K24" s="9">
+        <v>410.43</v>
+      </c>
+      <c r="L24" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.14361868924427726</v>
+      </c>
+      <c r="M24" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.10062434574547637</v>
+      </c>
+      <c r="N24" s="7">
+        <f t="shared" si="0"/>
+        <v>3.8117159044921065E-2</v>
+      </c>
+      <c r="T24" s="9">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="U24" s="9">
+        <v>655.23</v>
+      </c>
+      <c r="V24" s="9">
+        <v>427.7</v>
+      </c>
+      <c r="W24" s="7">
+        <f t="shared" si="3"/>
+        <v>-2.655771195097054E-2</v>
+      </c>
+      <c r="X24" s="7">
+        <f t="shared" si="1"/>
+        <v>-3.6166107913214E-2</v>
+      </c>
+      <c r="Y24" s="7">
+        <f t="shared" si="1"/>
+        <v>-2.5979322090819643E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="9:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="2">
+        <f>SUM(L22:L24)/3</f>
+        <v>-0.13800487341728476</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" ref="M25:N25" si="8">SUM(M22:M24)/3</f>
+        <v>-0.10131883039255019</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="8"/>
+        <v>3.3825182513731233E-2</v>
+      </c>
+      <c r="W25" s="13">
+        <f>SUM(W22:W24)/3</f>
+        <v>-3.4442360998061826E-2</v>
+      </c>
+      <c r="X25" s="13">
+        <f t="shared" ref="X25:Y25" si="9">SUM(X22:X24)/3</f>
+        <v>-6.0671531131118256E-2</v>
+      </c>
+      <c r="Y25" s="13">
+        <f t="shared" si="9"/>
+        <v>-2.2226999770763867E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="9:25" x14ac:dyDescent="0.25">
+      <c r="L27" s="15">
+        <f>SUM(L15,L20,L25)/3</f>
+        <v>-0.14642529186784273</v>
+      </c>
+      <c r="M27" s="15">
+        <f t="shared" ref="M27:N27" si="10">SUM(M15,M20,M25)/3</f>
+        <v>-0.13048066653653742</v>
+      </c>
+      <c r="N27" s="15">
+        <f t="shared" si="10"/>
+        <v>2.2461603574297606E-2</v>
+      </c>
+      <c r="W27" s="15">
+        <f>SUM(W15,W20,W25)/3</f>
+        <v>-3.8690399966099499E-2</v>
+      </c>
+      <c r="X27" s="15">
+        <f t="shared" ref="X27:Y27" si="11">SUM(X15,X20,X25)/3</f>
+        <v>-0.11009253438739663</v>
+      </c>
+      <c r="Y27" s="15">
+        <f t="shared" si="11"/>
+        <v>-6.249599964036448E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>